<commit_message>
Update drinks and admin
</commit_message>
<xml_diff>
--- a/data/drinks.xlsx
+++ b/data/drinks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mypc2\Desktop\GBS9\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A36C6E-B1C8-4266-AE50-97D23F1DA1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF31618-A5F9-487A-9BD3-6B876E9AFE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{85B9A84C-521F-415E-9407-6287BE1CC987}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{85B9A84C-521F-415E-9407-6287BE1CC987}"/>
   </bookViews>
   <sheets>
     <sheet name="Cocktails" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="309">
   <si>
     <t>No</t>
   </si>
@@ -874,6 +874,102 @@
   </si>
   <si>
     <t>cocktail-station-prepped.jpg</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Smirnoff</t>
+  </si>
+  <si>
+    <t>Gordons</t>
+  </si>
+  <si>
+    <t>Hendricks</t>
+  </si>
+  <si>
+    <t>Bacardi</t>
+  </si>
+  <si>
+    <t>Jameson</t>
+  </si>
+  <si>
+    <t>Powers</t>
+  </si>
+  <si>
+    <t>Guinness</t>
+  </si>
+  <si>
+    <t>Coors</t>
+  </si>
+  <si>
+    <t>Heineken</t>
+  </si>
+  <si>
+    <t>Smithwicks</t>
+  </si>
+  <si>
+    <t>Harp</t>
+  </si>
+  <si>
+    <t>Murphys</t>
+  </si>
+  <si>
+    <t>Beamish</t>
+  </si>
+  <si>
+    <t>Carlsberg</t>
+  </si>
+  <si>
+    <t>Coca Cola</t>
+  </si>
+  <si>
+    <t>Fanta Orange</t>
+  </si>
+  <si>
+    <t>Fanta Lemon</t>
+  </si>
+  <si>
+    <t>Club Lemon</t>
+  </si>
+  <si>
+    <t>Club Orange</t>
+  </si>
+  <si>
+    <t>7 Up</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>Tonic water</t>
+  </si>
+  <si>
+    <t>Schweppes Tonic</t>
+  </si>
+  <si>
+    <t>Schweppes Slimline Tonic</t>
+  </si>
+  <si>
+    <t>Slimline tonic</t>
+  </si>
+  <si>
+    <t>Ginger ale</t>
+  </si>
+  <si>
+    <t>Lucozade</t>
+  </si>
+  <si>
+    <t>Red Bull</t>
+  </si>
+  <si>
+    <t>Paddy</t>
+  </si>
+  <si>
+    <t>Hennessy</t>
+  </si>
+  <si>
+    <t>Huzzar</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1348,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2681,10 +2777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1DAADE-BA31-4DFD-A5C8-BF7FC49A43D1}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2712,6 +2808,51 @@
         <v>91</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>308</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2719,10 +2860,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4DA02F-846B-444F-B15E-6AB08FBC8131}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2742,6 +2883,46 @@
       </c>
       <c r="E1" s="4" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -2835,10 +3016,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E3F5C3-BC76-4BDF-809F-51355181FF25}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2857,6 +3038,76 @@
         <v>91</v>
       </c>
     </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2864,10 +3115,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44B94EE-BFDD-41BC-82DE-181F522B188E}">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2875,14 +3126,14 @@
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" customWidth="1"/>
-    <col min="8" max="10" width="18.140625" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="4" max="7" width="30.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
+    <col min="9" max="11" width="18.140625" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="60">
+    <row r="1" spans="1:21" ht="60">
       <c r="A1" s="2" t="s">
         <v>232</v>
       </c>
@@ -2902,49 +3153,52 @@
         <v>265</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="135">
+    <row r="2" spans="1:21" ht="135">
       <c r="A2" s="1" t="s">
         <v>258</v>
       </c>
@@ -2963,46 +3217,47 @@
       <c r="F2" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="105">
+    <row r="3" spans="1:21" ht="105">
       <c r="A3" s="1" t="s">
         <v>220</v>
       </c>
@@ -3017,41 +3272,42 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="1"/>
+      <c r="M3" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="R3" s="1" t="str">
-        <f>R2</f>
+      <c r="S3" s="1" t="str">
+        <f>S2</f>
         <v>/premium-listings.html</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="75">
+    <row r="4" spans="1:21" ht="75">
       <c r="A4" s="1" t="s">
         <v>226</v>
       </c>
@@ -3066,41 +3322,42 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="T4" s="5"/>
-    </row>
-    <row r="5" spans="1:20" ht="30">
+      <c r="U4" s="5"/>
+    </row>
+    <row r="5" spans="1:21" ht="30">
       <c r="A5" s="1" t="s">
         <v>252</v>
       </c>
@@ -3115,34 +3372,35 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="1"/>
+      <c r="M5" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3151,17 +3409,18 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="I6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="P6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="T6" s="5"/>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="S6" s="1"/>
+      <c r="U6" s="5"/>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -3170,16 +3429,17 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="P7" s="1"/>
       <c r="R7" s="1"/>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -3188,24 +3448,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="I8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="P8" s="1"/>
       <c r="R8" s="1"/>
-      <c r="T8" s="5"/>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="T10" s="5"/>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="S8" s="1"/>
+      <c r="U8" s="5"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="U10" s="5"/>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -3214,18 +3474,19 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="Q12" s="2"/>
+      <c r="P12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="T12" s="5"/>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="T14" s="5"/>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="T16" s="5"/>
-    </row>
-    <row r="18" spans="20:20">
-      <c r="T18" s="5"/>
+      <c r="S12" s="2"/>
+      <c r="U12" s="5"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="U14" s="5"/>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="U16" s="5"/>
+    </row>
+    <row r="18" spans="21:21">
+      <c r="U18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>